<commit_message>
Agregada la comparativa entre R y Python
</commit_message>
<xml_diff>
--- a/Reporte_Analisis_Zoo.xlsx
+++ b/Reporte_Analisis_Zoo.xlsx
@@ -33,19 +33,19 @@
     <t xml:space="preserve">n</t>
   </si>
   <si>
-    <t xml:space="preserve">August</t>
+    <t xml:space="preserve">agosto</t>
   </si>
   <si>
-    <t xml:space="preserve">September</t>
+    <t xml:space="preserve">septiembre</t>
   </si>
   <si>
-    <t xml:space="preserve">October</t>
+    <t xml:space="preserve">octubre</t>
   </si>
   <si>
-    <t xml:space="preserve">November</t>
+    <t xml:space="preserve">noviembre</t>
   </si>
   <si>
-    <t xml:space="preserve">December</t>
+    <t xml:space="preserve">diciembre</t>
   </si>
   <si>
     <t xml:space="preserve">Tabla: Distribución de Tipos de Hábitat</t>

</xml_diff>